<commit_message>
Refactor login users and use json
</commit_message>
<xml_diff>
--- a/TestResults.xlsx
+++ b/TestResults.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L265"/>
+  <dimension ref="A1:L266"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13337,6 +13337,68 @@
       <c r="L265" s="1" t="inlineStr">
         <is>
           <t>C:\Users\Fattal\Desktop\newTest\Fattal AutomationV1\Fattal_Tests\logs\test_mobile_booking_anonymous_user_2025-04-17_09-53-57.log</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_user</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>Test Description</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>2025-04-17 11:43:55</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>53.81s</t>
+        </is>
+      </c>
+      <c r="F266" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="G266" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="H266" t="inlineStr">
+        <is>
+          <t>חן טסט</t>
+        </is>
+      </c>
+      <c r="I266" t="inlineStr">
+        <is>
+          <t>chenttedgui@gmail.com</t>
+        </is>
+      </c>
+      <c r="J266" t="inlineStr">
+        <is>
+          <t>980023947</t>
+        </is>
+      </c>
+      <c r="K266" s="1" t="inlineStr">
+        <is>
+          <t>C:\Users\Fattal\Desktop\newTest\Fattal AutomationV1\Fattal_Tests\Screenshots\confirmation_PASS_2025-04-17_11-43-54.png</t>
+        </is>
+      </c>
+      <c r="L266" s="1" t="inlineStr">
+        <is>
+          <t>C:\Users\Fattal\Desktop\newTest\Fattal AutomationV1\Fattal_Tests\logs\test_mobile_booking_anonymous_user_2025-04-17_11-43-54.log</t>
         </is>
       </c>
     </row>
@@ -13868,6 +13930,8 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L264" r:id="rId524"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K265" r:id="rId525"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L265" r:id="rId526"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K266" r:id="rId527"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L266" r:id="rId528"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed dated picking IDS to set on November(Mobile)
</commit_message>
<xml_diff>
--- a/TestResults.xlsx
+++ b/TestResults.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2861,6 +2861,849 @@
       </c>
       <c r="N36" s="3" t="inlineStr"/>
       <c r="O36" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_join_fattal_and_friends</t>
+        </is>
+      </c>
+      <c r="B37" s="3" t="inlineStr"/>
+      <c r="C37" s="3" t="inlineStr"/>
+      <c r="D37" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי + הצטפרות למועדון</t>
+        </is>
+      </c>
+      <c r="E37" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F37" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 19:36:51</t>
+        </is>
+      </c>
+      <c r="G37" s="3" t="inlineStr">
+        <is>
+          <t>57.14s</t>
+        </is>
+      </c>
+      <c r="H37" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I37" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J37" s="3" t="inlineStr"/>
+      <c r="K37" s="3" t="inlineStr"/>
+      <c r="L37" s="3" t="inlineStr"/>
+      <c r="M37" s="3" t="inlineStr"/>
+      <c r="N37" s="3" t="inlineStr"/>
+      <c r="O37" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_join_fattal_and_friends</t>
+        </is>
+      </c>
+      <c r="B38" s="3" t="inlineStr"/>
+      <c r="C38" s="3" t="inlineStr"/>
+      <c r="D38" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי + הצטפרות למועדון</t>
+        </is>
+      </c>
+      <c r="E38" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F38" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 19:50:07</t>
+        </is>
+      </c>
+      <c r="G38" s="3" t="inlineStr">
+        <is>
+          <t>33.47s</t>
+        </is>
+      </c>
+      <c r="H38" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I38" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J38" s="3" t="inlineStr"/>
+      <c r="K38" s="3" t="inlineStr"/>
+      <c r="L38" s="3" t="inlineStr"/>
+      <c r="M38" s="3" t="inlineStr"/>
+      <c r="N38" s="3" t="inlineStr"/>
+      <c r="O38" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_join_fattal_and_friends</t>
+        </is>
+      </c>
+      <c r="B39" s="3" t="inlineStr"/>
+      <c r="C39" s="3" t="inlineStr"/>
+      <c r="D39" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי + הצטפרות למועדון</t>
+        </is>
+      </c>
+      <c r="E39" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F39" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 19:52:06</t>
+        </is>
+      </c>
+      <c r="G39" s="3" t="inlineStr">
+        <is>
+          <t>24.16s</t>
+        </is>
+      </c>
+      <c r="H39" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I39" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J39" s="3" t="inlineStr"/>
+      <c r="K39" s="3" t="inlineStr"/>
+      <c r="L39" s="3" t="inlineStr"/>
+      <c r="M39" s="3" t="inlineStr"/>
+      <c r="N39" s="3" t="inlineStr"/>
+      <c r="O39" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_join_fattal_and_friends</t>
+        </is>
+      </c>
+      <c r="B40" s="3" t="inlineStr"/>
+      <c r="C40" s="3" t="inlineStr"/>
+      <c r="D40" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי + הצטפרות למועדון</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F40" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 19:53:11</t>
+        </is>
+      </c>
+      <c r="G40" s="3" t="inlineStr">
+        <is>
+          <t>33.91s</t>
+        </is>
+      </c>
+      <c r="H40" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I40" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J40" s="3" t="inlineStr"/>
+      <c r="K40" s="3" t="inlineStr"/>
+      <c r="L40" s="3" t="inlineStr"/>
+      <c r="M40" s="3" t="inlineStr"/>
+      <c r="N40" s="3" t="inlineStr"/>
+      <c r="O40" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_join_fattal_and_friends</t>
+        </is>
+      </c>
+      <c r="B41" s="3" t="inlineStr"/>
+      <c r="C41" s="3" t="inlineStr"/>
+      <c r="D41" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי + הצטפרות למועדון</t>
+        </is>
+      </c>
+      <c r="E41" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F41" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 19:56:09</t>
+        </is>
+      </c>
+      <c r="G41" s="3" t="inlineStr">
+        <is>
+          <t>33.86s</t>
+        </is>
+      </c>
+      <c r="H41" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I41" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J41" s="3" t="inlineStr"/>
+      <c r="K41" s="3" t="inlineStr"/>
+      <c r="L41" s="3" t="inlineStr"/>
+      <c r="M41" s="3" t="inlineStr"/>
+      <c r="N41" s="3" t="inlineStr"/>
+      <c r="O41" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_join_fattal_and_friends</t>
+        </is>
+      </c>
+      <c r="B42" s="3" t="inlineStr"/>
+      <c r="C42" s="3" t="inlineStr"/>
+      <c r="D42" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי + הצטפרות למועדון</t>
+        </is>
+      </c>
+      <c r="E42" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F42" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:00:03</t>
+        </is>
+      </c>
+      <c r="G42" s="3" t="inlineStr">
+        <is>
+          <t>34.23s</t>
+        </is>
+      </c>
+      <c r="H42" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I42" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J42" s="3" t="inlineStr"/>
+      <c r="K42" s="3" t="inlineStr"/>
+      <c r="L42" s="3" t="inlineStr"/>
+      <c r="M42" s="3" t="inlineStr"/>
+      <c r="N42" s="3" t="inlineStr"/>
+      <c r="O42" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_join_fattal_and_friends</t>
+        </is>
+      </c>
+      <c r="B43" s="3" t="inlineStr"/>
+      <c r="C43" s="3" t="inlineStr"/>
+      <c r="D43" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי + הצטפרות למועדון</t>
+        </is>
+      </c>
+      <c r="E43" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F43" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:05:58</t>
+        </is>
+      </c>
+      <c r="G43" s="3" t="inlineStr">
+        <is>
+          <t>56.94s</t>
+        </is>
+      </c>
+      <c r="H43" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I43" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J43" s="3" t="inlineStr"/>
+      <c r="K43" s="3" t="inlineStr"/>
+      <c r="L43" s="3" t="inlineStr"/>
+      <c r="M43" s="3" t="inlineStr"/>
+      <c r="N43" s="3" t="inlineStr"/>
+      <c r="O43" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_join_fattal_and_friends</t>
+        </is>
+      </c>
+      <c r="B44" s="3" t="inlineStr"/>
+      <c r="C44" s="3" t="inlineStr"/>
+      <c r="D44" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי + הצטפרות למועדון</t>
+        </is>
+      </c>
+      <c r="E44" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F44" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:07:34</t>
+        </is>
+      </c>
+      <c r="G44" s="3" t="inlineStr">
+        <is>
+          <t>23.79s</t>
+        </is>
+      </c>
+      <c r="H44" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I44" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J44" s="3" t="inlineStr"/>
+      <c r="K44" s="3" t="inlineStr"/>
+      <c r="L44" s="3" t="inlineStr"/>
+      <c r="M44" s="3" t="inlineStr"/>
+      <c r="N44" s="3" t="inlineStr"/>
+      <c r="O44" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_join_fattal_and_friends</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="inlineStr"/>
+      <c r="C45" s="1" t="inlineStr">
+        <is>
+          <t>619746035</t>
+        </is>
+      </c>
+      <c r="D45" s="1" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי + הצטפרות למועדון</t>
+        </is>
+      </c>
+      <c r="E45" s="1" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="F45" s="1" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:12:07</t>
+        </is>
+      </c>
+      <c r="G45" s="1" t="inlineStr">
+        <is>
+          <t>117.99s</t>
+        </is>
+      </c>
+      <c r="H45" s="1" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I45" s="1" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J45" s="1" t="inlineStr">
+        <is>
+          <t>חן טסט</t>
+        </is>
+      </c>
+      <c r="K45" s="1" t="inlineStr">
+        <is>
+          <t>restestfattal@gmail.com</t>
+        </is>
+      </c>
+      <c r="L45" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="M45" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="N45" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O45" s="2" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_region_eilat</t>
+        </is>
+      </c>
+      <c r="B46" s="3" t="inlineStr"/>
+      <c r="C46" s="3" t="inlineStr"/>
+      <c r="D46" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי דרך אזור מלונות אילת</t>
+        </is>
+      </c>
+      <c r="E46" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F46" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:15:38</t>
+        </is>
+      </c>
+      <c r="G46" s="3" t="inlineStr">
+        <is>
+          <t>26.14s</t>
+        </is>
+      </c>
+      <c r="H46" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I46" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J46" s="3" t="inlineStr"/>
+      <c r="K46" s="3" t="inlineStr"/>
+      <c r="L46" s="3" t="inlineStr"/>
+      <c r="M46" s="3" t="inlineStr"/>
+      <c r="N46" s="3" t="inlineStr"/>
+      <c r="O46" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_region_eilat</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="inlineStr">
+        <is>
+          <t>980052161</t>
+        </is>
+      </c>
+      <c r="C47" s="1" t="inlineStr">
+        <is>
+          <t>798607867</t>
+        </is>
+      </c>
+      <c r="D47" s="1" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי דרך אזור מלונות אילת</t>
+        </is>
+      </c>
+      <c r="E47" s="1" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="F47" s="1" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:19:30</t>
+        </is>
+      </c>
+      <c r="G47" s="1" t="inlineStr">
+        <is>
+          <t>130.98s</t>
+        </is>
+      </c>
+      <c r="H47" s="1" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I47" s="1" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J47" s="1" t="inlineStr">
+        <is>
+          <t>חן טסט</t>
+        </is>
+      </c>
+      <c r="K47" s="1" t="inlineStr">
+        <is>
+          <t>restestfattal@gmail.com</t>
+        </is>
+      </c>
+      <c r="L47" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="M47" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="N47" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O47" s="2" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_region_eilat</t>
+        </is>
+      </c>
+      <c r="B48" s="3" t="inlineStr"/>
+      <c r="C48" s="3" t="inlineStr"/>
+      <c r="D48" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי דרך אזור מלונות אילת</t>
+        </is>
+      </c>
+      <c r="E48" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F48" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:21:56</t>
+        </is>
+      </c>
+      <c r="G48" s="3" t="inlineStr">
+        <is>
+          <t>23.62s</t>
+        </is>
+      </c>
+      <c r="H48" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I48" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J48" s="3" t="inlineStr"/>
+      <c r="K48" s="3" t="inlineStr"/>
+      <c r="L48" s="3" t="inlineStr"/>
+      <c r="M48" s="3" t="inlineStr"/>
+      <c r="N48" s="3" t="inlineStr"/>
+      <c r="O48" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_region_eilat</t>
+        </is>
+      </c>
+      <c r="B49" s="3" t="inlineStr"/>
+      <c r="C49" s="3" t="inlineStr"/>
+      <c r="D49" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי דרך אזור מלונות אילת</t>
+        </is>
+      </c>
+      <c r="E49" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F49" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:22:55</t>
+        </is>
+      </c>
+      <c r="G49" s="3" t="inlineStr">
+        <is>
+          <t>25.26s</t>
+        </is>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J49" s="3" t="inlineStr"/>
+      <c r="K49" s="3" t="inlineStr"/>
+      <c r="L49" s="3" t="inlineStr"/>
+      <c r="M49" s="3" t="inlineStr"/>
+      <c r="N49" s="3" t="inlineStr"/>
+      <c r="O49" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_region_eilat</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="inlineStr">
+        <is>
+          <t>980052162</t>
+        </is>
+      </c>
+      <c r="C50" s="1" t="inlineStr">
+        <is>
+          <t>788494219</t>
+        </is>
+      </c>
+      <c r="D50" s="1" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי דרך אזור מלונות אילת</t>
+        </is>
+      </c>
+      <c r="E50" s="1" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="F50" s="1" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:26:03</t>
+        </is>
+      </c>
+      <c r="G50" s="1" t="inlineStr">
+        <is>
+          <t>130.11s</t>
+        </is>
+      </c>
+      <c r="H50" s="1" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I50" s="1" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J50" s="1" t="inlineStr">
+        <is>
+          <t>חן טסט</t>
+        </is>
+      </c>
+      <c r="K50" s="1" t="inlineStr">
+        <is>
+          <t>restestfattal@gmail.com</t>
+        </is>
+      </c>
+      <c r="L50" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="M50" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="N50" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O50" s="2" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_user</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="inlineStr">
+        <is>
+          <t>980025886</t>
+        </is>
+      </c>
+      <c r="C51" s="1" t="inlineStr">
+        <is>
+          <t>329533012</t>
+        </is>
+      </c>
+      <c r="D51" s="1" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי</t>
+        </is>
+      </c>
+      <c r="E51" s="1" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="F51" s="1" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:30:11</t>
+        </is>
+      </c>
+      <c r="G51" s="1" t="inlineStr">
+        <is>
+          <t>74.79s</t>
+        </is>
+      </c>
+      <c r="H51" s="1" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I51" s="1" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J51" s="1" t="inlineStr">
+        <is>
+          <t>חן טסט</t>
+        </is>
+      </c>
+      <c r="K51" s="1" t="inlineStr">
+        <is>
+          <t>restestfattal@gmail.com</t>
+        </is>
+      </c>
+      <c r="L51" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="M51" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="N51" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O51" s="2" t="inlineStr">
         <is>
           <t>🧾 Log File</t>
         </is>
@@ -2965,6 +3808,33 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L36" r:id="rId95"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M36" r:id="rId96"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O36" r:id="rId97"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O37" r:id="rId98"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O38" r:id="rId99"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O39" r:id="rId100"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O40" r:id="rId101"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O41" r:id="rId102"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O42" r:id="rId103"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O43" r:id="rId104"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O44" r:id="rId105"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L45" r:id="rId106"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M45" r:id="rId107"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N45" r:id="rId108"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O45" r:id="rId109"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O46" r:id="rId110"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L47" r:id="rId111"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M47" r:id="rId112"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N47" r:id="rId113"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O47" r:id="rId114"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O48" r:id="rId115"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O49" r:id="rId116"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L50" r:id="rId117"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M50" r:id="rId118"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N50" r:id="rId119"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O50" r:id="rId120"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L51" r:id="rId121"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M51" r:id="rId122"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N51" r:id="rId123"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O51" r:id="rId124"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed WARpopup and Gift tests
</commit_message>
<xml_diff>
--- a/TestResults.xlsx
+++ b/TestResults.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3704,6 +3704,238 @@
         </is>
       </c>
       <c r="O51" s="2" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_club_member_eilat_with_flight</t>
+        </is>
+      </c>
+      <c r="B52" s="3" t="inlineStr"/>
+      <c r="C52" s="3" t="inlineStr">
+        <is>
+          <t>999318330</t>
+        </is>
+      </c>
+      <c r="D52" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש מחובר עם מועדון פעיל + טיסות</t>
+        </is>
+      </c>
+      <c r="E52" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F52" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:32:40</t>
+        </is>
+      </c>
+      <c r="G52" s="3" t="inlineStr">
+        <is>
+          <t>38.42s</t>
+        </is>
+      </c>
+      <c r="H52" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I52" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J52" s="3" t="inlineStr">
+        <is>
+          <t>Club User</t>
+        </is>
+      </c>
+      <c r="K52" s="3" t="inlineStr">
+        <is>
+          <t>restestfattal@gmail.com</t>
+        </is>
+      </c>
+      <c r="L52" s="3" t="inlineStr"/>
+      <c r="M52" s="3" t="inlineStr"/>
+      <c r="N52" s="3" t="inlineStr"/>
+      <c r="O52" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_club_member_eilat_with_flight</t>
+        </is>
+      </c>
+      <c r="B53" s="3" t="inlineStr"/>
+      <c r="C53" s="3" t="inlineStr">
+        <is>
+          <t>999318330</t>
+        </is>
+      </c>
+      <c r="D53" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש מחובר עם מועדון פעיל + טיסות</t>
+        </is>
+      </c>
+      <c r="E53" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F53" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:35:33</t>
+        </is>
+      </c>
+      <c r="G53" s="3" t="inlineStr">
+        <is>
+          <t>112.50s</t>
+        </is>
+      </c>
+      <c r="H53" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I53" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J53" s="3" t="inlineStr">
+        <is>
+          <t>Club User</t>
+        </is>
+      </c>
+      <c r="K53" s="3" t="inlineStr">
+        <is>
+          <t>restestfattal@gmail.com</t>
+        </is>
+      </c>
+      <c r="L53" s="3" t="inlineStr"/>
+      <c r="M53" s="3" t="inlineStr"/>
+      <c r="N53" s="3" t="inlineStr"/>
+      <c r="O53" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_club_member_eilat_with_flight</t>
+        </is>
+      </c>
+      <c r="B54" s="3" t="inlineStr"/>
+      <c r="C54" s="3" t="inlineStr">
+        <is>
+          <t>999318330</t>
+        </is>
+      </c>
+      <c r="D54" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש מחובר עם מועדון פעיל + טיסות</t>
+        </is>
+      </c>
+      <c r="E54" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F54" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:37:36</t>
+        </is>
+      </c>
+      <c r="G54" s="3" t="inlineStr">
+        <is>
+          <t>111.12s</t>
+        </is>
+      </c>
+      <c r="H54" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I54" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J54" s="3" t="inlineStr">
+        <is>
+          <t>Club User</t>
+        </is>
+      </c>
+      <c r="K54" s="3" t="inlineStr">
+        <is>
+          <t>restestfattal@gmail.com</t>
+        </is>
+      </c>
+      <c r="L54" s="3" t="inlineStr"/>
+      <c r="M54" s="3" t="inlineStr"/>
+      <c r="N54" s="3" t="inlineStr"/>
+      <c r="O54" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="inlineStr">
+        <is>
+          <t>test_mobile_booking_anonymous_user</t>
+        </is>
+      </c>
+      <c r="B55" s="3" t="inlineStr"/>
+      <c r="C55" s="3" t="inlineStr"/>
+      <c r="D55" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי</t>
+        </is>
+      </c>
+      <c r="E55" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F55" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:54:04</t>
+        </is>
+      </c>
+      <c r="G55" s="3" t="inlineStr">
+        <is>
+          <t>39.31s</t>
+        </is>
+      </c>
+      <c r="H55" s="3" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="I55" s="3" t="inlineStr">
+        <is>
+          <t>windows</t>
+        </is>
+      </c>
+      <c r="J55" s="3" t="inlineStr"/>
+      <c r="K55" s="3" t="inlineStr"/>
+      <c r="L55" s="3" t="inlineStr"/>
+      <c r="M55" s="3" t="inlineStr"/>
+      <c r="N55" s="3" t="inlineStr"/>
+      <c r="O55" s="4" t="inlineStr">
         <is>
           <t>🧾 Log File</t>
         </is>
@@ -3835,6 +4067,10 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M51" r:id="rId122"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N51" r:id="rId123"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O51" r:id="rId124"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O52" r:id="rId125"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O53" r:id="rId126"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O54" r:id="rId127"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O55" r:id="rId128"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed Desktop + warpopup
</commit_message>
<xml_diff>
--- a/TestResults.xlsx
+++ b/TestResults.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3936,6 +3936,657 @@
       <c r="M55" s="3" t="inlineStr"/>
       <c r="N55" s="3" t="inlineStr"/>
       <c r="O55" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="inlineStr">
+        <is>
+          <t>test_desktop_anonymous_booking</t>
+        </is>
+      </c>
+      <c r="B56" s="3" t="inlineStr"/>
+      <c r="C56" s="3" t="inlineStr"/>
+      <c r="D56" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה מתשמש אנונימי</t>
+        </is>
+      </c>
+      <c r="E56" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F56" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:56:47</t>
+        </is>
+      </c>
+      <c r="G56" s="3" t="inlineStr">
+        <is>
+          <t>46.64s</t>
+        </is>
+      </c>
+      <c r="H56" s="3" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="I56" s="3" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="J56" s="3" t="inlineStr"/>
+      <c r="K56" s="3" t="inlineStr"/>
+      <c r="L56" s="3" t="inlineStr"/>
+      <c r="M56" s="3" t="inlineStr"/>
+      <c r="N56" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O56" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="inlineStr">
+        <is>
+          <t>test_desktop_anonymous_booking</t>
+        </is>
+      </c>
+      <c r="B57" s="3" t="inlineStr"/>
+      <c r="C57" s="3" t="inlineStr"/>
+      <c r="D57" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה מתשמש אנונימי</t>
+        </is>
+      </c>
+      <c r="E57" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F57" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:59:03</t>
+        </is>
+      </c>
+      <c r="G57" s="3" t="inlineStr">
+        <is>
+          <t>45.53s</t>
+        </is>
+      </c>
+      <c r="H57" s="3" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="I57" s="3" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="J57" s="3" t="inlineStr"/>
+      <c r="K57" s="3" t="inlineStr"/>
+      <c r="L57" s="3" t="inlineStr"/>
+      <c r="M57" s="3" t="inlineStr"/>
+      <c r="N57" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O57" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="inlineStr">
+        <is>
+          <t>test_desktop_anonymous_booking</t>
+        </is>
+      </c>
+      <c r="B58" s="3" t="inlineStr"/>
+      <c r="C58" s="3" t="inlineStr"/>
+      <c r="D58" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה מתשמש אנונימי</t>
+        </is>
+      </c>
+      <c r="E58" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F58" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 20:59:56</t>
+        </is>
+      </c>
+      <c r="G58" s="3" t="inlineStr">
+        <is>
+          <t>46.07s</t>
+        </is>
+      </c>
+      <c r="H58" s="3" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="I58" s="3" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="J58" s="3" t="inlineStr"/>
+      <c r="K58" s="3" t="inlineStr"/>
+      <c r="L58" s="3" t="inlineStr"/>
+      <c r="M58" s="3" t="inlineStr"/>
+      <c r="N58" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O58" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="inlineStr">
+        <is>
+          <t>test_desktop_anonymous_booking</t>
+        </is>
+      </c>
+      <c r="B59" s="3" t="inlineStr"/>
+      <c r="C59" s="3" t="inlineStr"/>
+      <c r="D59" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה מתשמש אנונימי</t>
+        </is>
+      </c>
+      <c r="E59" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F59" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 21:02:23</t>
+        </is>
+      </c>
+      <c r="G59" s="3" t="inlineStr">
+        <is>
+          <t>45.85s</t>
+        </is>
+      </c>
+      <c r="H59" s="3" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="I59" s="3" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="J59" s="3" t="inlineStr"/>
+      <c r="K59" s="3" t="inlineStr"/>
+      <c r="L59" s="3" t="inlineStr"/>
+      <c r="M59" s="3" t="inlineStr"/>
+      <c r="N59" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O59" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="3" t="inlineStr">
+        <is>
+          <t>test_desktop_anonymous_booking</t>
+        </is>
+      </c>
+      <c r="B60" s="3" t="inlineStr"/>
+      <c r="C60" s="3" t="inlineStr"/>
+      <c r="D60" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה מתשמש אנונימי</t>
+        </is>
+      </c>
+      <c r="E60" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F60" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 21:05:38</t>
+        </is>
+      </c>
+      <c r="G60" s="3" t="inlineStr">
+        <is>
+          <t>45.38s</t>
+        </is>
+      </c>
+      <c r="H60" s="3" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="I60" s="3" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="J60" s="3" t="inlineStr"/>
+      <c r="K60" s="3" t="inlineStr"/>
+      <c r="L60" s="3" t="inlineStr"/>
+      <c r="M60" s="3" t="inlineStr"/>
+      <c r="N60" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O60" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="inlineStr">
+        <is>
+          <t>test_desktop_anonymous_booking</t>
+        </is>
+      </c>
+      <c r="B61" s="3" t="inlineStr"/>
+      <c r="C61" s="3" t="inlineStr"/>
+      <c r="D61" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה מתשמש אנונימי</t>
+        </is>
+      </c>
+      <c r="E61" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F61" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 21:07:08</t>
+        </is>
+      </c>
+      <c r="G61" s="3" t="inlineStr">
+        <is>
+          <t>29.67s</t>
+        </is>
+      </c>
+      <c r="H61" s="3" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="I61" s="3" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="J61" s="3" t="inlineStr"/>
+      <c r="K61" s="3" t="inlineStr"/>
+      <c r="L61" s="3" t="inlineStr"/>
+      <c r="M61" s="3" t="inlineStr"/>
+      <c r="N61" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O61" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="3" t="inlineStr">
+        <is>
+          <t>test_desktop_anonymous_booking</t>
+        </is>
+      </c>
+      <c r="B62" s="3" t="inlineStr"/>
+      <c r="C62" s="3" t="inlineStr">
+        <is>
+          <t>256898768</t>
+        </is>
+      </c>
+      <c r="D62" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה מתשמש אנונימי</t>
+        </is>
+      </c>
+      <c r="E62" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F62" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 21:08:25</t>
+        </is>
+      </c>
+      <c r="G62" s="3" t="inlineStr">
+        <is>
+          <t>39.39s</t>
+        </is>
+      </c>
+      <c r="H62" s="3" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="I62" s="3" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="J62" s="3" t="inlineStr"/>
+      <c r="K62" s="3" t="inlineStr"/>
+      <c r="L62" s="3" t="inlineStr"/>
+      <c r="M62" s="3" t="inlineStr"/>
+      <c r="N62" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O62" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="3" t="inlineStr">
+        <is>
+          <t>test_desktop_anonymous_booking</t>
+        </is>
+      </c>
+      <c r="B63" s="3" t="inlineStr"/>
+      <c r="C63" s="3" t="inlineStr">
+        <is>
+          <t>888438629</t>
+        </is>
+      </c>
+      <c r="D63" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה מתשמש אנונימי</t>
+        </is>
+      </c>
+      <c r="E63" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F63" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 21:13:41</t>
+        </is>
+      </c>
+      <c r="G63" s="3" t="inlineStr">
+        <is>
+          <t>38.18s</t>
+        </is>
+      </c>
+      <c r="H63" s="3" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="I63" s="3" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="J63" s="3" t="inlineStr"/>
+      <c r="K63" s="3" t="inlineStr"/>
+      <c r="L63" s="3" t="inlineStr"/>
+      <c r="M63" s="3" t="inlineStr"/>
+      <c r="N63" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O63" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="3" t="inlineStr">
+        <is>
+          <t>test_desktop_anonymous_booking</t>
+        </is>
+      </c>
+      <c r="B64" s="3" t="inlineStr"/>
+      <c r="C64" s="3" t="inlineStr">
+        <is>
+          <t>503517476</t>
+        </is>
+      </c>
+      <c r="D64" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה מתשמש אנונימי</t>
+        </is>
+      </c>
+      <c r="E64" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F64" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 21:15:37</t>
+        </is>
+      </c>
+      <c r="G64" s="3" t="inlineStr">
+        <is>
+          <t>52.71s</t>
+        </is>
+      </c>
+      <c r="H64" s="3" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="I64" s="3" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="J64" s="3" t="inlineStr">
+        <is>
+          <t>חן טסט</t>
+        </is>
+      </c>
+      <c r="K64" s="3" t="inlineStr">
+        <is>
+          <t>restestfattal@gmail.com</t>
+        </is>
+      </c>
+      <c r="L64" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="M64" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="N64" s="3" t="inlineStr"/>
+      <c r="O64" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="3" t="inlineStr">
+        <is>
+          <t>test_desktop_booking_anonymous_region_eilat</t>
+        </is>
+      </c>
+      <c r="B65" s="3" t="inlineStr"/>
+      <c r="C65" s="3" t="inlineStr">
+        <is>
+          <t>794085886</t>
+        </is>
+      </c>
+      <c r="D65" s="3" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה משתמש אנונימי דרך אזור מלונות אילת</t>
+        </is>
+      </c>
+      <c r="E65" s="3" t="inlineStr">
+        <is>
+          <t>FAILED</t>
+        </is>
+      </c>
+      <c r="F65" s="3" t="inlineStr">
+        <is>
+          <t>2025-08-30 21:17:29</t>
+        </is>
+      </c>
+      <c r="G65" s="3" t="inlineStr">
+        <is>
+          <t>106.01s</t>
+        </is>
+      </c>
+      <c r="H65" s="3" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="I65" s="3" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="J65" s="3" t="inlineStr">
+        <is>
+          <t>חן טסט</t>
+        </is>
+      </c>
+      <c r="K65" s="3" t="inlineStr">
+        <is>
+          <t>restestfattal@gmail.com</t>
+        </is>
+      </c>
+      <c r="L65" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="M65" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="N65" s="4" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O65" s="4" t="inlineStr">
+        <is>
+          <t>🧾 Log File</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="inlineStr">
+        <is>
+          <t>test_desktop_anonymous_booking</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="inlineStr">
+        <is>
+          <t>980025889</t>
+        </is>
+      </c>
+      <c r="C66" s="1" t="inlineStr">
+        <is>
+          <t>435686373</t>
+        </is>
+      </c>
+      <c r="D66" s="1" t="inlineStr">
+        <is>
+          <t>בדיקת השלמת הזמנה מתשמש אנונימי</t>
+        </is>
+      </c>
+      <c r="E66" s="1" t="inlineStr">
+        <is>
+          <t>PASSED</t>
+        </is>
+      </c>
+      <c r="F66" s="1" t="inlineStr">
+        <is>
+          <t>2025-08-30 21:22:34</t>
+        </is>
+      </c>
+      <c r="G66" s="1" t="inlineStr">
+        <is>
+          <t>69.46s</t>
+        </is>
+      </c>
+      <c r="H66" s="1" t="inlineStr">
+        <is>
+          <t>chrome</t>
+        </is>
+      </c>
+      <c r="I66" s="1" t="inlineStr">
+        <is>
+          <t>Windows</t>
+        </is>
+      </c>
+      <c r="J66" s="1" t="inlineStr">
+        <is>
+          <t>חן טסט</t>
+        </is>
+      </c>
+      <c r="K66" s="1" t="inlineStr">
+        <is>
+          <t>restestfattal@gmail.com</t>
+        </is>
+      </c>
+      <c r="L66" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="M66" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="N66" s="2" t="inlineStr">
+        <is>
+          <t>📷 Screenshot</t>
+        </is>
+      </c>
+      <c r="O66" s="2" t="inlineStr">
         <is>
           <t>🧾 Log File</t>
         </is>
@@ -4071,6 +4722,33 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O53" r:id="rId126"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O54" r:id="rId127"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O55" r:id="rId128"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N56" r:id="rId129"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O56" r:id="rId130"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N57" r:id="rId131"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O57" r:id="rId132"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N58" r:id="rId133"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O58" r:id="rId134"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N59" r:id="rId135"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O59" r:id="rId136"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N60" r:id="rId137"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O60" r:id="rId138"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N61" r:id="rId139"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O61" r:id="rId140"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N62" r:id="rId141"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O62" r:id="rId142"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N63" r:id="rId143"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O63" r:id="rId144"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L64" r:id="rId145"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M64" r:id="rId146"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O64" r:id="rId147"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L65" r:id="rId148"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M65" r:id="rId149"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N65" r:id="rId150"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O65" r:id="rId151"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="L66" r:id="rId152"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M66" r:id="rId153"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="N66" r:id="rId154"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="O66" r:id="rId155"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>